<commit_message>
Small changes to format
</commit_message>
<xml_diff>
--- a/PROJECT/PM/GanttChart_3_Semester.xlsx
+++ b/PROJECT/PM/GanttChart_3_Semester.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1BD04E-BDF9-42E7-8A36-D42123F26BF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{3E1BD04E-BDF9-42E7-8A36-D42123F26BF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C638E5DD-58DD-4E85-B94E-33E0A0B01028}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,12 +146,6 @@
     <t>Fragenaustausch mit dem Kunden</t>
   </si>
   <si>
-    <t>Woche 1 Sprint</t>
-  </si>
-  <si>
-    <t>Woche 5 Sprint</t>
-  </si>
-  <si>
     <t>Firmenname : DHBW-Gruppe 4</t>
   </si>
   <si>
@@ -206,12 +200,6 @@
     <t>Präsentation fertigstellen</t>
   </si>
   <si>
-    <t>Woche 8 Sprint</t>
-  </si>
-  <si>
-    <t>Woche 7 Sprint</t>
-  </si>
-  <si>
     <t>Überprüfung CRS</t>
   </si>
   <si>
@@ -225,6 +213,18 @@
   </si>
   <si>
     <t>Überprüfung SAS</t>
+  </si>
+  <si>
+    <t>Ab Woche 1</t>
+  </si>
+  <si>
+    <t>Ab Woche 5</t>
+  </si>
+  <si>
+    <t>Ab Woche 8</t>
+  </si>
+  <si>
+    <t>Ab Woche 7</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1189,10 @@
     <xf numFmtId="167" fontId="9" fillId="45" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="42" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1204,10 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="42" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1765,7 +1765,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1801,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I2" s="29"/>
     </row>
@@ -1810,110 +1810,110 @@
         <v>2</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="79">
         <v>44463</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="79"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="77"/>
+      <c r="B4" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="78"/>
       <c r="D4" s="54" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="74">
+      <c r="I4" s="75">
         <f>I5</f>
         <v>44466</v>
       </c>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="74">
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="75">
         <f>P5</f>
         <v>44473</v>
       </c>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="74">
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="75">
         <f>W5</f>
         <v>44480</v>
       </c>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
-      <c r="AA4" s="75"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="74">
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="77"/>
+      <c r="AD4" s="75">
         <f>AD5</f>
         <v>44487</v>
       </c>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="74">
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="77"/>
+      <c r="AK4" s="75">
         <f>AK5</f>
         <v>44494</v>
       </c>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75"/>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="75"/>
-      <c r="AP4" s="75"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="74">
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="77"/>
+      <c r="AR4" s="75">
         <f>AR5</f>
         <v>44501</v>
       </c>
-      <c r="AS4" s="75"/>
-      <c r="AT4" s="75"/>
-      <c r="AU4" s="75"/>
-      <c r="AV4" s="75"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="76"/>
-      <c r="AY4" s="74">
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="75">
         <f>AY5</f>
         <v>44508</v>
       </c>
-      <c r="AZ4" s="75"/>
-      <c r="BA4" s="75"/>
-      <c r="BB4" s="75"/>
-      <c r="BC4" s="75"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="76"/>
-      <c r="BF4" s="74">
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="77"/>
+      <c r="BF4" s="75">
         <f>BF5</f>
         <v>44515</v>
       </c>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="75"/>
-      <c r="BI4" s="75"/>
-      <c r="BJ4" s="75"/>
-      <c r="BK4" s="75"/>
-      <c r="BL4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="77"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
@@ -2470,7 +2470,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="15"/>
@@ -2546,7 +2546,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
@@ -2626,7 +2626,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="16">
         <v>1</v>
@@ -2699,10 +2699,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="16">
         <v>1</v>
@@ -2777,10 +2777,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="71">
         <v>1</v>
@@ -2857,7 +2857,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="66"/>
@@ -2928,10 +2928,10 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="26"/>
       <c r="B14" s="69" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="71">
         <v>0.1</v>
@@ -3007,10 +3007,10 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="26"/>
       <c r="B15" s="69" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="70" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="71">
         <v>0</v>
@@ -3083,10 +3083,10 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
       <c r="B16" s="69" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="71">
         <v>0</v>
@@ -3164,7 +3164,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="18"/>
@@ -3235,12 +3235,12 @@
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="78">
+        <v>39</v>
+      </c>
+      <c r="D18" s="73">
         <v>0</v>
       </c>
       <c r="E18" s="45">
@@ -3314,7 +3314,7 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="26"/>
       <c r="B19" s="59" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C19" s="60"/>
       <c r="D19" s="61"/>
@@ -3382,12 +3382,12 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
       <c r="B20" s="57" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="79">
+        <v>34</v>
+      </c>
+      <c r="D20" s="74">
         <v>0</v>
       </c>
       <c r="E20" s="58">
@@ -3458,12 +3458,12 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="26"/>
       <c r="B21" s="57" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="79">
+        <v>33</v>
+      </c>
+      <c r="D21" s="74">
         <v>0</v>
       </c>
       <c r="E21" s="58">
@@ -3534,12 +3534,12 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26"/>
       <c r="B22" s="57" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="79">
+        <v>40</v>
+      </c>
+      <c r="D22" s="74">
         <v>0</v>
       </c>
       <c r="E22" s="58">
@@ -3610,12 +3610,12 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="26"/>
       <c r="B23" s="57" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="79">
+        <v>35</v>
+      </c>
+      <c r="D23" s="74">
         <v>0</v>
       </c>
       <c r="E23" s="58">
@@ -3686,12 +3686,12 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="26"/>
       <c r="B24" s="57" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C24" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="79">
+        <v>37</v>
+      </c>
+      <c r="D24" s="74">
         <v>0</v>
       </c>
       <c r="E24" s="58">
@@ -3762,12 +3762,12 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26"/>
       <c r="B25" s="57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="79">
+        <v>39</v>
+      </c>
+      <c r="D25" s="74">
         <v>0</v>
       </c>
       <c r="E25" s="58">
@@ -3920,16 +3920,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D9 D19 D26 D11:D17">
     <cfRule type="dataBar" priority="24">

</xml_diff>